<commit_message>
removed German words from excel
</commit_message>
<xml_diff>
--- a/RaR Bands.xlsx
+++ b/RaR Bands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeller/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeller/sources/r/rar-bands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5485FA47-B271-404E-B5D9-8D1F9A893BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC60AB69-A33F-1D4C-AD64-48199E947B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{EF0E05CA-8964-4548-AE1A-A427DD16F240}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="142">
   <si>
     <t>Die Ärtze</t>
   </si>
@@ -248,18 +248,12 @@
     <t>true</t>
   </si>
   <si>
-    <t>weiblich</t>
-  </si>
-  <si>
     <t>Danger Dan</t>
   </si>
   <si>
     <t>Ingo Donot</t>
   </si>
   <si>
-    <t>männlich</t>
-  </si>
-  <si>
     <t>M. Shadows</t>
   </si>
   <si>
@@ -462,6 +456,15 @@
   </si>
   <si>
     <t>band_age</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -837,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D32184-8F25-E947-B158-8977D47A576A}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70:I70"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,28 +859,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
         <v>138</v>
       </c>
-      <c r="B1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" t="s">
-        <v>140</v>
-      </c>
       <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>134</v>
-      </c>
-      <c r="G1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -905,7 +908,7 @@
         <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -923,7 +926,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>1981</v>
@@ -933,7 +936,7 @@
         <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -961,7 +964,7 @@
         <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -979,7 +982,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F5">
         <v>1992</v>
@@ -989,7 +992,7 @@
         <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1007,7 +1010,7 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6">
         <v>1969</v>
@@ -1017,7 +1020,7 @@
         <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1035,7 +1038,7 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7">
         <v>1967</v>
@@ -1045,7 +1048,7 @@
         <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1060,7 +1063,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>1973</v>
@@ -1070,7 +1073,7 @@
         <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1085,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F9">
         <v>1970</v>
@@ -1095,7 +1098,7 @@
         <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1110,13 +1113,13 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1131,13 +1134,13 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1152,7 +1155,7 @@
         <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F12">
         <v>1963</v>
@@ -1162,7 +1165,7 @@
         <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1177,7 +1180,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F13">
         <v>1986</v>
@@ -1187,7 +1190,7 @@
         <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1202,13 +1205,13 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F14">
         <v>1990</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1233,7 +1236,7 @@
         <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1248,13 +1251,13 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1279,7 +1282,7 @@
         <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1294,7 +1297,7 @@
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F18">
         <v>1994</v>
@@ -1304,7 +1307,7 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1319,7 +1322,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F19">
         <v>1965</v>
@@ -1329,7 +1332,7 @@
         <v>59</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1344,7 +1347,7 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F20">
         <v>1986</v>
@@ -1354,7 +1357,7 @@
         <v>38</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1369,7 +1372,7 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F21">
         <v>1990</v>
@@ -1379,7 +1382,7 @@
         <v>34</v>
       </c>
       <c r="H21" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1394,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F22">
         <v>1997</v>
@@ -1404,7 +1407,7 @@
         <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1419,7 +1422,7 @@
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F23">
         <v>1967</v>
@@ -1429,7 +1432,7 @@
         <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1444,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F24">
         <v>1978</v>
@@ -1454,7 +1457,7 @@
         <v>46</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1469,7 +1472,7 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F25">
         <v>1997</v>
@@ -1479,7 +1482,7 @@
         <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1504,7 +1507,7 @@
         <v>52</v>
       </c>
       <c r="H26" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1519,7 +1522,7 @@
         <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F27">
         <v>1979</v>
@@ -1529,7 +1532,7 @@
         <v>45</v>
       </c>
       <c r="H27" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1544,7 +1547,7 @@
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F28">
         <v>1975</v>
@@ -1554,7 +1557,7 @@
         <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1569,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F29">
         <v>1997</v>
@@ -1579,7 +1582,7 @@
         <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1594,7 +1597,7 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F30">
         <v>1995</v>
@@ -1604,7 +1607,7 @@
         <v>29</v>
       </c>
       <c r="H30" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1619,7 +1622,7 @@
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F31">
         <v>1985</v>
@@ -1629,7 +1632,7 @@
         <v>39</v>
       </c>
       <c r="H31" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1644,7 +1647,7 @@
         <v>36</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F32">
         <v>1970</v>
@@ -1654,7 +1657,7 @@
         <v>54</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1669,7 +1672,7 @@
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F33">
         <v>1995</v>
@@ -1679,7 +1682,7 @@
         <v>29</v>
       </c>
       <c r="H33" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1694,7 +1697,7 @@
         <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34">
         <v>1983</v>
@@ -1704,7 +1707,7 @@
         <v>41</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1719,7 +1722,7 @@
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F35">
         <v>1968</v>
@@ -1729,7 +1732,7 @@
         <v>56</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1744,7 +1747,7 @@
         <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36">
         <v>1976</v>
@@ -1754,7 +1757,7 @@
         <v>48</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1779,7 +1782,7 @@
         <v>21</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1794,7 +1797,7 @@
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F38">
         <v>1978</v>
@@ -1804,7 +1807,7 @@
         <v>46</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1819,7 +1822,7 @@
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F39">
         <v>1982</v>
@@ -1829,7 +1832,7 @@
         <v>42</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1844,7 +1847,7 @@
         <v>22</v>
       </c>
       <c r="E40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40">
         <v>1982</v>
@@ -1854,7 +1857,7 @@
         <v>42</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1869,9 +1872,9 @@
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41">
+        <v>104</v>
+      </c>
+      <c r="F41" s="4">
         <v>1997</v>
       </c>
       <c r="G41">
@@ -1879,7 +1882,7 @@
         <v>27</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1894,7 +1897,7 @@
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F42">
         <v>1984</v>
@@ -1904,7 +1907,7 @@
         <v>40</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1919,13 +1922,13 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1940,13 +1943,13 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1961,7 +1964,7 @@
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F45">
         <v>1979</v>
@@ -1971,7 +1974,7 @@
         <v>45</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1986,13 +1989,13 @@
         <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2007,13 +2010,13 @@
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2028,7 +2031,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F48">
         <v>1973</v>
@@ -2038,7 +2041,7 @@
         <v>51</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2053,7 +2056,7 @@
         <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F49">
         <v>1983</v>
@@ -2063,7 +2066,7 @@
         <v>41</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2078,7 +2081,7 @@
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F50">
         <v>1999</v>
@@ -2088,7 +2091,7 @@
         <v>25</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2103,7 +2106,7 @@
         <v>21</v>
       </c>
       <c r="E51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F51">
         <v>1982</v>
@@ -2113,7 +2116,7 @@
         <v>42</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2128,7 +2131,7 @@
         <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F52">
         <v>1989</v>
@@ -2138,7 +2141,7 @@
         <v>35</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2163,7 +2166,7 @@
         <v>51</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2178,7 +2181,7 @@
         <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F54">
         <v>1967</v>
@@ -2188,7 +2191,7 @@
         <v>57</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2203,7 +2206,7 @@
         <v>26</v>
       </c>
       <c r="E55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F55">
         <v>1983</v>
@@ -2213,7 +2216,7 @@
         <v>41</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2228,7 +2231,7 @@
         <v>37</v>
       </c>
       <c r="E56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F56">
         <v>1969</v>
@@ -2238,7 +2241,7 @@
         <v>55</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2253,13 +2256,13 @@
         <v>19</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F57">
         <v>1990</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2274,7 +2277,7 @@
         <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F58">
         <v>1958</v>
@@ -2284,7 +2287,7 @@
         <v>66</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2299,7 +2302,7 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F59">
         <v>1991</v>
@@ -2309,7 +2312,7 @@
         <v>33</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2324,7 +2327,7 @@
         <v>35</v>
       </c>
       <c r="E60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F60">
         <v>1966</v>
@@ -2334,7 +2337,7 @@
         <v>58</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2349,7 +2352,7 @@
         <v>20</v>
       </c>
       <c r="E61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F61">
         <v>1981</v>
@@ -2359,12 +2362,12 @@
         <v>43</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C62">
         <v>2010</v>
@@ -2374,7 +2377,7 @@
         <v>14</v>
       </c>
       <c r="E62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F62" s="4">
         <v>1992</v>
@@ -2384,7 +2387,7 @@
         <v>32</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2399,7 +2402,7 @@
         <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F63">
         <v>1988</v>
@@ -2409,7 +2412,7 @@
         <v>36</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2424,7 +2427,7 @@
         <v>14</v>
       </c>
       <c r="E64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F64">
         <v>1993</v>
@@ -2434,7 +2437,7 @@
         <v>31</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2449,7 +2452,7 @@
         <v>18</v>
       </c>
       <c r="E65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F65">
         <v>1990</v>
@@ -2459,7 +2462,7 @@
         <v>34</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2474,7 +2477,7 @@
         <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F66">
         <v>1987</v>
@@ -2484,7 +2487,7 @@
         <v>37</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2499,7 +2502,7 @@
         <v>18</v>
       </c>
       <c r="E67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F67">
         <v>1984</v>
@@ -2509,10 +2512,16 @@
         <v>40</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>